<commit_message>
lab04: update stack trace spread sheet
</commit_message>
<xml_diff>
--- a/Lab04/stack-trace.xlsx
+++ b/Lab04/stack-trace.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a5f3d3ccdac3f129/Programming/repos/ceg3310-assignments/Lab04/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeesmithh\repos\ceg3310-assignments\Lab04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="8_{C53BD075-2888-4398-8F79-53B072D9C3CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5251B527-9BB9-427E-9E5A-5E115A41E8CF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C4F456-0E88-47B9-B44B-F55D42541290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{A3CACB95-ADD9-42EA-A377-70DB2BAD29D7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A3CACB95-ADD9-42EA-A377-70DB2BAD29D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="34">
   <si>
     <t>main() return address</t>
   </si>
@@ -99,6 +99,45 @@
   </si>
   <si>
     <t>int product</t>
+  </si>
+  <si>
+    <t>array[0]</t>
+  </si>
+  <si>
+    <t>array[4]</t>
+  </si>
+  <si>
+    <t>array[3]</t>
+  </si>
+  <si>
+    <t>array[2]</t>
+  </si>
+  <si>
+    <t>array[1]</t>
+  </si>
+  <si>
+    <t>x0002</t>
+  </si>
+  <si>
+    <t>x0003</t>
+  </si>
+  <si>
+    <t>x0001</t>
+  </si>
+  <si>
+    <t>array pointer param</t>
+  </si>
+  <si>
+    <t>arraySize param</t>
+  </si>
+  <si>
+    <t>main()</t>
+  </si>
+  <si>
+    <t>sumOfSquares(int a[], int arraySize)</t>
+  </si>
+  <si>
+    <t>square(int x)</t>
   </si>
 </sst>
 </file>
@@ -134,8 +173,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -473,15 +515,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE34279-D803-4DB1-874E-658A728EF49E}">
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="139" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81:F96"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N81" sqref="N81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="9" max="9" width="29" customWidth="1"/>
+    <col min="10" max="10" width="31.28515625" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -868,103 +914,118 @@
         <v>5FDC</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f t="shared" ref="A65:A89" si="1">DEC2HEX(HEX2DEC(A66)-1)</f>
         <v>5FDD</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f t="shared" si="1"/>
         <v>5FDE</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f t="shared" si="1"/>
         <v>5FDF</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f t="shared" si="1"/>
         <v>5FE0</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f t="shared" si="1"/>
         <v>5FE1</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f t="shared" si="1"/>
         <v>5FE2</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f t="shared" si="1"/>
         <v>5FE3</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f t="shared" si="1"/>
         <v>5FE4</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f t="shared" si="1"/>
         <v>5FE5</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f t="shared" si="1"/>
         <v>5FE6</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f t="shared" si="1"/>
         <v>5FE7</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f t="shared" si="1"/>
         <v>5FE8</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f t="shared" si="1"/>
         <v>5FE9</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="J77" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
         <f t="shared" si="1"/>
         <v>5FEA</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I78" t="s">
+        <v>20</v>
+      </c>
+      <c r="J78" s="2"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f t="shared" si="1"/>
         <v>5FEB</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I79" t="s">
+        <v>5</v>
+      </c>
+      <c r="J79" s="2"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f t="shared" si="1"/>
         <v>5FEC</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I80" t="s">
+        <v>4</v>
+      </c>
+      <c r="J80" s="2"/>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
         <f t="shared" si="1"/>
         <v>5FED</v>
@@ -972,8 +1033,18 @@
       <c r="C81" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I81" t="s">
+        <v>1</v>
+      </c>
+      <c r="J81" s="2"/>
+      <c r="K81" t="s">
+        <v>13</v>
+      </c>
+      <c r="L81" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
         <f t="shared" si="1"/>
         <v>5FEE</v>
@@ -981,8 +1052,18 @@
       <c r="C82" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I82" t="s">
+        <v>19</v>
+      </c>
+      <c r="J82" s="2"/>
+      <c r="K82" t="s">
+        <v>16</v>
+      </c>
+      <c r="L82" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
         <f t="shared" si="1"/>
         <v>5FEF</v>
@@ -990,8 +1071,14 @@
       <c r="C83" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I83" t="s">
+        <v>17</v>
+      </c>
+      <c r="J83" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
         <f t="shared" si="1"/>
         <v>5FF0</v>
@@ -1005,8 +1092,12 @@
       <c r="E84" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I84" t="s">
+        <v>11</v>
+      </c>
+      <c r="J84" s="2"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
         <f t="shared" si="1"/>
         <v>5FF1</v>
@@ -1020,8 +1111,15 @@
       <c r="E85" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H85" t="s">
+        <v>18</v>
+      </c>
+      <c r="I85" t="s">
+        <v>7</v>
+      </c>
+      <c r="J85" s="2"/>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
         <f t="shared" si="1"/>
         <v>5FF2</v>
@@ -1029,8 +1127,12 @@
       <c r="C86" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I86" t="s">
+        <v>5</v>
+      </c>
+      <c r="J86" s="2"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
         <f t="shared" si="1"/>
         <v>5FF3</v>
@@ -1038,8 +1140,12 @@
       <c r="C87" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I87" t="s">
+        <v>4</v>
+      </c>
+      <c r="J87" s="2"/>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
         <f t="shared" si="1"/>
         <v>5FF4</v>
@@ -1050,8 +1156,21 @@
       <c r="C88" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H88" t="s">
+        <v>3</v>
+      </c>
+      <c r="I88" t="s">
+        <v>1</v>
+      </c>
+      <c r="J88" s="2"/>
+      <c r="K88" t="s">
+        <v>13</v>
+      </c>
+      <c r="L88" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
         <f t="shared" si="1"/>
         <v>5FF5</v>
@@ -1059,8 +1178,18 @@
       <c r="C89" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I89" t="s">
+        <v>2</v>
+      </c>
+      <c r="J89" s="2"/>
+      <c r="K89" t="s">
+        <v>16</v>
+      </c>
+      <c r="L89" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
         <f t="shared" ref="A90:A98" si="2">DEC2HEX(HEX2DEC(A91)-1)</f>
         <v>5FF6</v>
@@ -1068,8 +1197,14 @@
       <c r="C90" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I90" t="s">
+        <v>29</v>
+      </c>
+      <c r="J90" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="str">
         <f t="shared" si="2"/>
         <v>5FF7</v>
@@ -1086,8 +1221,15 @@
       <c r="E91" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H91" t="s">
+        <v>6</v>
+      </c>
+      <c r="I91" t="s">
+        <v>30</v>
+      </c>
+      <c r="J91" s="2"/>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" t="str">
         <f t="shared" si="2"/>
         <v>5FF8</v>
@@ -1101,8 +1243,15 @@
       <c r="E92" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H92" t="s">
+        <v>28</v>
+      </c>
+      <c r="I92" t="s">
+        <v>21</v>
+      </c>
+      <c r="J92" s="2"/>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
         <f t="shared" si="2"/>
         <v>5FF9</v>
@@ -1110,8 +1259,15 @@
       <c r="C93" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H93" t="s">
+        <v>18</v>
+      </c>
+      <c r="I93" t="s">
+        <v>25</v>
+      </c>
+      <c r="J93" s="2"/>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" t="str">
         <f t="shared" si="2"/>
         <v>5FFA</v>
@@ -1122,8 +1278,15 @@
       <c r="C94" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H94" t="s">
+        <v>6</v>
+      </c>
+      <c r="I94" t="s">
+        <v>24</v>
+      </c>
+      <c r="J94" s="2"/>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
         <f t="shared" si="2"/>
         <v>5FFB</v>
@@ -1131,8 +1294,15 @@
       <c r="C95" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H95" t="s">
+        <v>27</v>
+      </c>
+      <c r="I95" t="s">
+        <v>23</v>
+      </c>
+      <c r="J95" s="2"/>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" t="str">
         <f t="shared" si="2"/>
         <v>5FFC</v>
@@ -1143,8 +1313,15 @@
       <c r="C96" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H96" t="s">
+        <v>26</v>
+      </c>
+      <c r="I96" t="s">
+        <v>22</v>
+      </c>
+      <c r="J96" s="2"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
         <f t="shared" si="2"/>
         <v>5FFD</v>
@@ -1152,8 +1329,12 @@
       <c r="C97" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I97" t="s">
+        <v>8</v>
+      </c>
+      <c r="J97" s="2"/>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
         <f t="shared" si="2"/>
         <v>5FFE</v>
@@ -1167,8 +1348,18 @@
       <c r="E98" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I98" t="s">
+        <v>1</v>
+      </c>
+      <c r="J98" s="2"/>
+      <c r="K98" t="s">
+        <v>13</v>
+      </c>
+      <c r="L98" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
         <f>DEC2HEX(HEX2DEC(A100)-1)</f>
         <v>5FFF</v>
@@ -1182,13 +1373,28 @@
       <c r="E99" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I99" t="s">
+        <v>0</v>
+      </c>
+      <c r="J99" s="2"/>
+      <c r="K99" t="s">
+        <v>16</v>
+      </c>
+      <c r="L99" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>6000</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="J77:J82"/>
+    <mergeCell ref="J83:J89"/>
+    <mergeCell ref="J90:J99"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
lab04: final completed lab
</commit_message>
<xml_diff>
--- a/Lab04/stack-trace.xlsx
+++ b/Lab04/stack-trace.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeesmithh\repos\ceg3310-assignments\Lab04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C4F456-0E88-47B9-B44B-F55D42541290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122CC9CB-5ED1-482F-859B-ADE0DC054C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A3CACB95-ADD9-42EA-A377-70DB2BAD29D7}"/>
+    <workbookView xWindow="-1095" yWindow="5175" windowWidth="21600" windowHeight="11295" xr2:uid="{A3CACB95-ADD9-42EA-A377-70DB2BAD29D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>main() return address</t>
   </si>
@@ -65,18 +65,9 @@
     <t>int total</t>
   </si>
   <si>
-    <t>int array[]</t>
-  </si>
-  <si>
-    <t>param arraySize (taken from global)</t>
-  </si>
-  <si>
     <t>int sum</t>
   </si>
   <si>
-    <t>param array[] (first address)</t>
-  </si>
-  <si>
     <t>R5</t>
   </si>
   <si>
@@ -125,19 +116,13 @@
     <t>x0001</t>
   </si>
   <si>
-    <t>array pointer param</t>
-  </si>
-  <si>
-    <t>arraySize param</t>
-  </si>
-  <si>
-    <t>main()</t>
-  </si>
-  <si>
-    <t>sumOfSquares(int a[], int arraySize)</t>
-  </si>
-  <si>
-    <t>square(int x)</t>
+    <t>array parameter</t>
+  </si>
+  <si>
+    <t>arraySize parameter</t>
+  </si>
+  <si>
+    <t>x5FF9</t>
   </si>
 </sst>
 </file>
@@ -173,11 +158,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -515,19 +497,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE34279-D803-4DB1-874E-658A728EF49E}">
-  <dimension ref="A1:L100"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N81" sqref="N81"/>
+      <selection activeCell="B78" sqref="B78:F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="31.140625" customWidth="1"/>
     <col min="9" max="9" width="29" customWidth="1"/>
-    <col min="10" max="10" width="31.28515625" customWidth="1"/>
-    <col min="12" max="12" width="21.5703125" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -914,360 +895,274 @@
         <v>5FDC</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f t="shared" ref="A65:A89" si="1">DEC2HEX(HEX2DEC(A66)-1)</f>
         <v>5FDD</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f t="shared" si="1"/>
         <v>5FDE</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f t="shared" si="1"/>
         <v>5FDF</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f t="shared" si="1"/>
         <v>5FE0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f t="shared" si="1"/>
         <v>5FE1</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f t="shared" si="1"/>
         <v>5FE2</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f t="shared" si="1"/>
         <v>5FE3</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f t="shared" si="1"/>
         <v>5FE4</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f t="shared" si="1"/>
         <v>5FE5</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f t="shared" si="1"/>
         <v>5FE6</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f t="shared" si="1"/>
         <v>5FE7</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f t="shared" si="1"/>
         <v>5FE8</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f t="shared" si="1"/>
         <v>5FE9</v>
       </c>
-      <c r="J77" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
         <f t="shared" si="1"/>
         <v>5FEA</v>
       </c>
-      <c r="I78" t="s">
-        <v>20</v>
-      </c>
-      <c r="J78" s="2"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f t="shared" si="1"/>
         <v>5FEB</v>
       </c>
-      <c r="I79" t="s">
+      <c r="C79" t="s">
         <v>5</v>
       </c>
-      <c r="J79" s="2"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f t="shared" si="1"/>
         <v>5FEC</v>
       </c>
-      <c r="I80" t="s">
+      <c r="C80" t="s">
         <v>4</v>
       </c>
-      <c r="J80" s="2"/>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
         <f t="shared" si="1"/>
         <v>5FED</v>
       </c>
       <c r="C81" t="s">
-        <v>20</v>
-      </c>
-      <c r="I81" t="s">
         <v>1</v>
       </c>
-      <c r="J81" s="2"/>
-      <c r="K81" t="s">
+      <c r="D81" t="s">
+        <v>10</v>
+      </c>
+      <c r="E81" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="str">
+        <f t="shared" si="1"/>
+        <v>5FEE</v>
+      </c>
+      <c r="C82" t="s">
+        <v>16</v>
+      </c>
+      <c r="D82" t="s">
         <v>13</v>
       </c>
-      <c r="L81" t="s">
+      <c r="E82" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="str">
+        <f t="shared" si="1"/>
+        <v>5FEF</v>
+      </c>
+      <c r="C83" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A82" t="str">
-        <f t="shared" si="1"/>
-        <v>5FEE</v>
-      </c>
-      <c r="C82" t="s">
-        <v>5</v>
-      </c>
-      <c r="I82" t="s">
-        <v>19</v>
-      </c>
-      <c r="J82" s="2"/>
-      <c r="K82" t="s">
-        <v>16</v>
-      </c>
-      <c r="L82" t="s">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="str">
+        <f t="shared" si="1"/>
+        <v>5FF0</v>
+      </c>
+      <c r="B84" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A83" t="str">
-        <f t="shared" si="1"/>
-        <v>5FEF</v>
-      </c>
-      <c r="C83" t="s">
+      <c r="C84" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="str">
+        <f t="shared" si="1"/>
+        <v>5FF1</v>
+      </c>
+      <c r="C85" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="str">
+        <f t="shared" si="1"/>
+        <v>5FF2</v>
+      </c>
+      <c r="C86" t="s">
         <v>4</v>
       </c>
-      <c r="I83" t="s">
-        <v>17</v>
-      </c>
-      <c r="J83" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A84" t="str">
-        <f t="shared" si="1"/>
-        <v>5FF0</v>
-      </c>
-      <c r="C84" t="s">
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="str">
+        <f t="shared" si="1"/>
+        <v>5FF3</v>
+      </c>
+      <c r="B87" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87" t="s">
         <v>1</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D87" t="s">
+        <v>10</v>
+      </c>
+      <c r="E87" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="str">
+        <f t="shared" si="1"/>
+        <v>5FF4</v>
+      </c>
+      <c r="C88" t="s">
+        <v>2</v>
+      </c>
+      <c r="D88" t="s">
         <v>13</v>
       </c>
-      <c r="E84" t="s">
-        <v>14</v>
-      </c>
-      <c r="I84" t="s">
-        <v>11</v>
-      </c>
-      <c r="J84" s="2"/>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A85" t="str">
-        <f t="shared" si="1"/>
-        <v>5FF1</v>
-      </c>
-      <c r="C85" t="s">
-        <v>19</v>
-      </c>
-      <c r="D85" t="s">
-        <v>16</v>
-      </c>
-      <c r="E85" t="s">
-        <v>15</v>
-      </c>
-      <c r="H85" t="s">
-        <v>18</v>
-      </c>
-      <c r="I85" t="s">
-        <v>7</v>
-      </c>
-      <c r="J85" s="2"/>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A86" t="str">
-        <f t="shared" si="1"/>
-        <v>5FF2</v>
-      </c>
-      <c r="C86" t="s">
-        <v>17</v>
-      </c>
-      <c r="I86" t="s">
-        <v>5</v>
-      </c>
-      <c r="J86" s="2"/>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A87" t="str">
-        <f t="shared" si="1"/>
-        <v>5FF3</v>
-      </c>
-      <c r="C87" t="s">
-        <v>11</v>
-      </c>
-      <c r="I87" t="s">
-        <v>4</v>
-      </c>
-      <c r="J87" s="2"/>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A88" t="str">
-        <f t="shared" si="1"/>
-        <v>5FF4</v>
-      </c>
-      <c r="B88" t="s">
-        <v>18</v>
-      </c>
-      <c r="C88" t="s">
-        <v>7</v>
-      </c>
-      <c r="H88" t="s">
-        <v>3</v>
-      </c>
-      <c r="I88" t="s">
-        <v>1</v>
-      </c>
-      <c r="J88" s="2"/>
-      <c r="K88" t="s">
-        <v>13</v>
-      </c>
-      <c r="L88" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E88" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
         <f t="shared" si="1"/>
         <v>5FF5</v>
       </c>
+      <c r="B89" t="s">
+        <v>6</v>
+      </c>
       <c r="C89" t="s">
-        <v>5</v>
-      </c>
-      <c r="I89" t="s">
-        <v>2</v>
-      </c>
-      <c r="J89" s="2"/>
-      <c r="K89" t="s">
-        <v>16</v>
-      </c>
-      <c r="L89" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
         <f t="shared" ref="A90:A98" si="2">DEC2HEX(HEX2DEC(A91)-1)</f>
         <v>5FF6</v>
       </c>
+      <c r="B90" t="s">
+        <v>28</v>
+      </c>
       <c r="C90" t="s">
-        <v>4</v>
-      </c>
-      <c r="I90" t="s">
-        <v>29</v>
-      </c>
-      <c r="J90" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="str">
         <f t="shared" si="2"/>
         <v>5FF7</v>
       </c>
       <c r="B91" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C91" t="s">
-        <v>1</v>
-      </c>
-      <c r="D91" t="s">
-        <v>13</v>
-      </c>
-      <c r="E91" t="s">
-        <v>14</v>
-      </c>
-      <c r="H91" t="s">
-        <v>6</v>
-      </c>
-      <c r="I91" t="s">
-        <v>30</v>
-      </c>
-      <c r="J91" s="2"/>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="str">
         <f t="shared" si="2"/>
         <v>5FF8</v>
       </c>
+      <c r="B92" t="s">
+        <v>23</v>
+      </c>
       <c r="C92" t="s">
-        <v>2</v>
-      </c>
-      <c r="D92" t="s">
-        <v>16</v>
-      </c>
-      <c r="E92" t="s">
-        <v>15</v>
-      </c>
-      <c r="H92" t="s">
-        <v>28</v>
-      </c>
-      <c r="I92" t="s">
-        <v>21</v>
-      </c>
-      <c r="J92" s="2"/>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
         <f t="shared" si="2"/>
         <v>5FF9</v>
       </c>
+      <c r="B93" t="s">
+        <v>24</v>
+      </c>
       <c r="C93" t="s">
-        <v>12</v>
-      </c>
-      <c r="H93" t="s">
-        <v>18</v>
-      </c>
-      <c r="I93" t="s">
-        <v>25</v>
-      </c>
-      <c r="J93" s="2"/>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="str">
         <f t="shared" si="2"/>
         <v>5FFA</v>
@@ -1276,125 +1171,81 @@
         <v>6</v>
       </c>
       <c r="C94" t="s">
-        <v>10</v>
-      </c>
-      <c r="H94" t="s">
-        <v>6</v>
-      </c>
-      <c r="I94" t="s">
-        <v>24</v>
-      </c>
-      <c r="J94" s="2"/>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
         <f t="shared" si="2"/>
         <v>5FFB</v>
       </c>
+      <c r="B95" t="s">
+        <v>15</v>
+      </c>
       <c r="C95" t="s">
-        <v>8</v>
-      </c>
-      <c r="H95" t="s">
-        <v>27</v>
-      </c>
-      <c r="I95" t="s">
-        <v>23</v>
-      </c>
-      <c r="J95" s="2"/>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="str">
         <f t="shared" si="2"/>
         <v>5FFC</v>
       </c>
       <c r="B96" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C96" t="s">
-        <v>9</v>
-      </c>
-      <c r="H96" t="s">
-        <v>26</v>
-      </c>
-      <c r="I96" t="s">
-        <v>22</v>
-      </c>
-      <c r="J96" s="2"/>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
         <f t="shared" si="2"/>
         <v>5FFD</v>
       </c>
       <c r="C97" t="s">
-        <v>4</v>
-      </c>
-      <c r="I97" t="s">
-        <v>8</v>
-      </c>
-      <c r="J97" s="2"/>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
         <f t="shared" si="2"/>
         <v>5FFE</v>
       </c>
       <c r="C98" t="s">
-        <v>1</v>
-      </c>
-      <c r="D98" t="s">
-        <v>13</v>
-      </c>
-      <c r="E98" t="s">
-        <v>14</v>
-      </c>
-      <c r="I98" t="s">
-        <v>1</v>
-      </c>
-      <c r="J98" s="2"/>
-      <c r="K98" t="s">
-        <v>13</v>
-      </c>
-      <c r="L98" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
         <f>DEC2HEX(HEX2DEC(A100)-1)</f>
         <v>5FFF</v>
       </c>
       <c r="C99" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D99" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E99" t="s">
-        <v>15</v>
-      </c>
-      <c r="I99" t="s">
-        <v>0</v>
-      </c>
-      <c r="J99" s="2"/>
-      <c r="K99" t="s">
-        <v>16</v>
-      </c>
-      <c r="L99" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>6000</v>
       </c>
+      <c r="C100" t="s">
+        <v>0</v>
+      </c>
+      <c r="D100" t="s">
+        <v>13</v>
+      </c>
+      <c r="E100" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="J77:J82"/>
-    <mergeCell ref="J83:J89"/>
-    <mergeCell ref="J90:J99"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
lab04: update stack trace spreadsheet to match assembly code
</commit_message>
<xml_diff>
--- a/Lab04/stack-trace.xlsx
+++ b/Lab04/stack-trace.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeesmithh\repos\ceg3310-assignments\Lab04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122CC9CB-5ED1-482F-859B-ADE0DC054C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317FD7A5-47C8-412F-8B3A-9CCA297DDF19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1095" yWindow="5175" windowWidth="21600" windowHeight="11295" xr2:uid="{A3CACB95-ADD9-42EA-A377-70DB2BAD29D7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A3CACB95-ADD9-42EA-A377-70DB2BAD29D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>main() return address</t>
   </si>
@@ -500,7 +500,7 @@
   <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78:F100"/>
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,109 +895,100 @@
         <v>5FDC</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f t="shared" ref="A65:A89" si="1">DEC2HEX(HEX2DEC(A66)-1)</f>
         <v>5FDD</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f t="shared" si="1"/>
         <v>5FDE</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f t="shared" si="1"/>
         <v>5FDF</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f t="shared" si="1"/>
         <v>5FE0</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f t="shared" si="1"/>
         <v>5FE1</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f t="shared" si="1"/>
         <v>5FE2</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f t="shared" si="1"/>
         <v>5FE3</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f t="shared" si="1"/>
         <v>5FE4</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f t="shared" si="1"/>
         <v>5FE5</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f t="shared" si="1"/>
         <v>5FE6</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f t="shared" si="1"/>
         <v>5FE7</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f t="shared" si="1"/>
         <v>5FE8</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f t="shared" si="1"/>
         <v>5FE9</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
         <f t="shared" si="1"/>
         <v>5FEA</v>
       </c>
-      <c r="C78" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f t="shared" si="1"/>
         <v>5FEB</v>
       </c>
-      <c r="C79" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f t="shared" si="1"/>
         <v>5FEC</v>
-      </c>
-      <c r="C80" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -1006,13 +997,7 @@
         <v>5FED</v>
       </c>
       <c r="C81" t="s">
-        <v>1</v>
-      </c>
-      <c r="D81" t="s">
-        <v>10</v>
-      </c>
-      <c r="E81" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -1021,13 +1006,7 @@
         <v>5FEE</v>
       </c>
       <c r="C82" t="s">
-        <v>16</v>
-      </c>
-      <c r="D82" t="s">
-        <v>13</v>
-      </c>
-      <c r="E82" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -1036,7 +1015,7 @@
         <v>5FEF</v>
       </c>
       <c r="C83" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -1044,11 +1023,14 @@
         <f t="shared" si="1"/>
         <v>5FF0</v>
       </c>
-      <c r="B84" t="s">
-        <v>15</v>
-      </c>
       <c r="C84" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="D84" t="s">
+        <v>10</v>
+      </c>
+      <c r="E84" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -1057,7 +1039,13 @@
         <v>5FF1</v>
       </c>
       <c r="C85" t="s">
-        <v>7</v>
+        <v>16</v>
+      </c>
+      <c r="D85" t="s">
+        <v>13</v>
+      </c>
+      <c r="E85" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -1066,7 +1054,7 @@
         <v>5FF2</v>
       </c>
       <c r="C86" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -1075,16 +1063,10 @@
         <v>5FF3</v>
       </c>
       <c r="B87" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C87" t="s">
-        <v>1</v>
-      </c>
-      <c r="D87" t="s">
-        <v>10</v>
-      </c>
-      <c r="E87" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -1093,13 +1075,7 @@
         <v>5FF4</v>
       </c>
       <c r="C88" t="s">
-        <v>2</v>
-      </c>
-      <c r="D88" t="s">
-        <v>13</v>
-      </c>
-      <c r="E88" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -1107,11 +1083,8 @@
         <f t="shared" si="1"/>
         <v>5FF5</v>
       </c>
-      <c r="B89" t="s">
-        <v>6</v>
-      </c>
       <c r="C89" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -1120,10 +1093,16 @@
         <v>5FF6</v>
       </c>
       <c r="B90" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="C90" t="s">
-        <v>26</v>
+        <v>1</v>
+      </c>
+      <c r="D90" t="s">
+        <v>10</v>
+      </c>
+      <c r="E90" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -1131,11 +1110,14 @@
         <f t="shared" si="2"/>
         <v>5FF7</v>
       </c>
-      <c r="B91" t="s">
-        <v>25</v>
-      </c>
       <c r="C91" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="D91" t="s">
+        <v>13</v>
+      </c>
+      <c r="E91" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -1144,10 +1126,10 @@
         <v>5FF8</v>
       </c>
       <c r="B92" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C92" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -1156,10 +1138,10 @@
         <v>5FF9</v>
       </c>
       <c r="B93" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C93" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -1168,10 +1150,10 @@
         <v>5FFA</v>
       </c>
       <c r="B94" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C94" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -1180,10 +1162,10 @@
         <v>5FFB</v>
       </c>
       <c r="B95" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C95" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -1192,10 +1174,10 @@
         <v>5FFC</v>
       </c>
       <c r="B96" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C96" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -1203,8 +1185,11 @@
         <f t="shared" si="2"/>
         <v>5FFD</v>
       </c>
+      <c r="B97" t="s">
+        <v>6</v>
+      </c>
       <c r="C97" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -1212,8 +1197,11 @@
         <f t="shared" si="2"/>
         <v>5FFE</v>
       </c>
+      <c r="B98" t="s">
+        <v>15</v>
+      </c>
       <c r="C98" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -1221,14 +1209,11 @@
         <f>DEC2HEX(HEX2DEC(A100)-1)</f>
         <v>5FFF</v>
       </c>
+      <c r="B99" t="s">
+        <v>25</v>
+      </c>
       <c r="C99" t="s">
-        <v>1</v>
-      </c>
-      <c r="D99" t="s">
-        <v>10</v>
-      </c>
-      <c r="E99" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -1239,10 +1224,10 @@
         <v>0</v>
       </c>
       <c r="D100" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E100" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>